<commit_message>
Fixed NaNs remaining in platform QC join table
</commit_message>
<xml_diff>
--- a/example_summary_spreadsheet.xlsx
+++ b/example_summary_spreadsheet.xlsx
@@ -7,16 +7,29 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary statistics report" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FC + output per experiment" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 plot" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Run data output plot" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Starting active pores plot" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Flow cells per experiment plot" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Output per experiment plot" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Output per flow cell plot" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pores vs. data output" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pores vs. read N50" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 vs. data output" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Output per flow cell ID" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FC + output per experiment" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 plot" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Run data output plot" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Starting active pores plot" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Flow cells per experiment plot" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Output per experiment plot" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Output per flow cell plot" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform QC active pores plot" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform-seq pore diff plot" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform-seq time diff plot" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pores vs. data output" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pores vs. read N50" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 vs. data output" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. starting active pores" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. pore difference" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore vs. time difference" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference vs. run output" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output pore diff" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output starting pores" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform QC pores over time" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference over time" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Run output over time" sheetId="24" state="visible" r:id="rId24"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -189,6 +202,306 @@
 </wsDr>
 </file>
 
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8153400" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8029575" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8153400" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8277225" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8277225" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8277225" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8153400" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8191500" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8191500" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8467725" cy="6991350"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
@@ -219,6 +532,66 @@
 </wsDr>
 </file>
 
+<file path=xl/drawings/drawing20.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8467725" cy="6991350"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing21.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8153400" cy="6991350"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
@@ -348,7 +721,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9144000" cy="6858000"/>
+    <ext cx="12192000" cy="9144000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -378,7 +751,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9144000" cy="6858000"/>
+    <ext cx="12192000" cy="9144000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -408,7 +781,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9144000" cy="6858000"/>
+    <ext cx="12192000" cy="9144000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -718,7 +1091,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -855,144 +1228,200 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Flow cells per experiment</t>
+          <t>Platform QC active pores</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>5120</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>8684</v>
       </c>
       <c r="E5" t="n">
-        <v>1.020833333333333</v>
+        <v>7167.52</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>7504</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>8684</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1443375672974064</v>
+        <v>968.900068806548</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Flow cell output (Gb)</t>
+          <t>Pore difference</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="C6" t="n">
-        <v>18.653</v>
+        <v>55</v>
       </c>
       <c r="D6" t="n">
-        <v>105.651</v>
+        <v>3751</v>
       </c>
       <c r="E6" t="n">
-        <v>60.48742857142857</v>
+        <v>731.6799999999999</v>
       </c>
       <c r="F6" t="n">
-        <v>64.84</v>
+        <v>576</v>
       </c>
       <c r="G6" t="n">
-        <v>70.04000000000001</v>
+        <v>657</v>
       </c>
       <c r="H6" t="n">
-        <v>23.57373106429414</v>
+        <v>706.0248295917078</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Total experiment output (Gb)</t>
+          <t>Flow cells per experiment</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>48</v>
       </c>
       <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.020833333333333</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.1443375672974064</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Flow cell output (Gb)</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>49</v>
+      </c>
+      <c r="C8" t="n">
         <v>18.653</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D8" t="n">
         <v>105.651</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E8" t="n">
+        <v>60.48742857142857</v>
+      </c>
+      <c r="F8" t="n">
+        <v>64.84</v>
+      </c>
+      <c r="G8" t="n">
+        <v>70.04000000000001</v>
+      </c>
+      <c r="H8" t="n">
+        <v>23.57373106429414</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Total experiment output (Gb)</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>48</v>
+      </c>
+      <c r="C9" t="n">
+        <v>18.653</v>
+      </c>
+      <c r="D9" t="n">
+        <v>105.651</v>
+      </c>
+      <c r="E9" t="n">
         <v>61.74758333333333</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F9" t="n">
         <v>65.8455</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G9" t="n">
         <v>51.4</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H9" t="n">
         <v>23.22835168480337</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
         <is>
           <t>Flow Cells</t>
         </is>
       </c>
-      <c r="B9" s="1" t="inlineStr">
+      <c r="B11" s="1" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>1</v>
-      </c>
-      <c r="B10" t="n">
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" t="n">
         <v>47</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="n">
+    <row r="13">
+      <c r="A13" t="n">
         <v>2</v>
       </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
         <is>
           <t>MinKNOW Version</t>
         </is>
       </c>
-      <c r="B13" s="1" t="inlineStr">
+      <c r="B15" s="1" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+    <row r="16">
+      <c r="A16" t="inlineStr">
         <is>
           <t>22.10.7</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="B16" t="n">
         <v>29</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
+    <row r="17">
+      <c r="A17" t="inlineStr">
         <is>
           <t>23.11.7</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="B17" t="n">
         <v>20</v>
       </c>
     </row>
@@ -1039,7 +1468,1025 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Flow Cell ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Flow cell output (Gb)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Top up</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>PAK70026</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>70.04000000000001</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>PAK81672</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>44.76</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>PAK81747</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>64.88800000000001</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>PAM03576</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>62.739</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>PAM03900</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>81.72</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>PAO12997</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>72.068</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>PAO13048</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>40.146</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>PAO20010</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>67.571</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>PAO39054</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>66.803</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>PAO48090</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>72.812</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>PAO55546</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>59.537</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>PAO91787</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>25.545</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>PAO94913</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>43.133</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>PAO96644</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>67.64700000000001</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>PAO96952</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>48.245</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>PAO98839</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>64.84</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>PAO99671</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>94.875</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>PAO99819</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>67.61199999999999</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>PAQ00427</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>56.438</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>PAQ01363</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>22.841</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>PAQ02677</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>97.884</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>PAQ08189</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>52.964</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>PAQ08471</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>70.066</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>PAQ10380</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>58.45</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>PAQ74172</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>60.801</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Top up</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>PAQ82297</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>82.56699999999999</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>PAS31662</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>69.38500000000001</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>PAS32187</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>51.4</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>PAS44637</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>71.89400000000001</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>PAS45694</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>105.651</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>PAS45697</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>20.304</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Top up</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>PAS45828</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>18.653</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Top up</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>PAS46448</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>30.907</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Top up</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>PAS46764</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>31.548</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Top up</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>PAS62242</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>34.276</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Top up</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>PAS64255</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>36.085</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Top up</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>PAS65568</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>28.677</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Top up</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>PAU32242</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>79.541</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>PAU38820</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>95.88</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>PAU53616</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>98.765</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>PAU54572</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>42.787</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>PAU54613</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>86.95999999999999</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>PAU56778</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>64.33</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>PAU70344</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>26.084</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Top up</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>PAW05746</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>24.709</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>PAW17248</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>80.19799999999999</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>PAW19784</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>72.258</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>PAW25364</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>76.652</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>PAW28552</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>99.94799999999999</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Initial run</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1696,25 +3143,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated JSON parser with flow cell position and run ISO timestamp
</commit_message>
<xml_diff>
--- a/example_summary_spreadsheet.xlsx
+++ b/example_summary_spreadsheet.xlsx
@@ -21,15 +21,16 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pores vs. data output" sheetId="13" state="visible" r:id="rId13"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pores vs. read N50" sheetId="14" state="visible" r:id="rId14"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 vs. data output" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. starting active pores" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. pore difference" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore vs. time difference" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference vs. run output" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output pore diff" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output starting pores" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform QC pores over time" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference over time" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Run output over time" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 vs. data no line" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. starting active pores" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. pore difference" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore vs. time difference" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference vs. run output" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output pore diff" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output starting pores" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform QC pores over time" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference over time" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Run output over time" sheetId="25" state="visible" r:id="rId25"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -301,7 +302,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8277225" cy="6457950"/>
+    <ext cx="8153400" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -391,7 +392,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8153400" cy="6457950"/>
+    <ext cx="8277225" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -421,7 +422,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8191500" cy="6457950"/>
+    <ext cx="8153400" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -481,7 +482,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8467725" cy="6991350"/>
+    <ext cx="8191500" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -563,6 +564,36 @@
 </file>
 
 <file path=xl/drawings/drawing21.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8467725" cy="6991350"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing22.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -2486,6 +2517,25 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Updated example data and outputs with newest report parser.
</commit_message>
<xml_diff>
--- a/example_summary_spreadsheet.xlsx
+++ b/example_summary_spreadsheet.xlsx
@@ -452,7 +452,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8191500" cy="6457950"/>
+    <ext cx="8153400" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -482,7 +482,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8191500" cy="6457950"/>
+    <ext cx="8153400" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -1182,22 +1182,22 @@
         <v>49</v>
       </c>
       <c r="C2" t="n">
-        <v>25.15</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>51.38</v>
+        <v>33.2</v>
       </c>
       <c r="E2" t="n">
-        <v>32.45918367346939</v>
+        <v>12.3234693877551</v>
       </c>
       <c r="F2" t="n">
-        <v>32.08</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>33.2</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>4.087696904908015</v>
+        <v>15.06547467874539</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Reran test case from tutorial
</commit_message>
<xml_diff>
--- a/example_summary_spreadsheet.xlsx
+++ b/example_summary_spreadsheet.xlsx
@@ -11,26 +11,30 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FC + output per experiment" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 plot" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Run data output plot" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Starting active pores plot" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Flow cells per experiment plot" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Output per experiment plot" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Output per flow cell plot" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform QC active pores plot" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform-seq pore diff plot" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform-seq time diff plot" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pores vs. data output" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pores vs. read N50" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 vs. data output" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 vs. data no line" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. starting active pores" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. pore difference" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore vs. time difference" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference vs. run output" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output pore diff" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output starting pores" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform QC pores over time" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference over time" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Run output over time" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Run read count plot" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Starting active pores plot" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Flow cells per experiment plot" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Output per experiment plot" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Output per flow cell plot" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform QC active pores plot" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform-seq pore diff plot" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform-seq time diff plot" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pores vs. data output" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pores vs. read count" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pores vs. read N50" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 vs. data output" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 vs. data no line" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 vs. read count" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 vs. count no line" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. starting active pores" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. pore difference" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore vs. time difference" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference vs. run output" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output pore diff" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output starting pores" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform QC pores over time" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference over time" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Run output over time" sheetId="29" state="visible" r:id="rId29"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -182,7 +186,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="12192000" cy="9144000"/>
+    <ext cx="9915525" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -204,6 +208,36 @@
 </file>
 
 <file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="9915525" cy="8648700"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -233,7 +267,37 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="7905750" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -263,7 +327,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -293,7 +357,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -323,7 +387,67 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="7905750" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="7905750" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -353,7 +477,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -383,7 +507,37 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="9915525" cy="8648700"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing20.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -413,7 +567,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing21.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -443,7 +597,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing22.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -452,7 +606,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8153400" cy="6457950"/>
+    <ext cx="8191500" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -473,7 +627,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing23.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -482,7 +636,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8153400" cy="6457950"/>
+    <ext cx="8191500" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -503,37 +657,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="12192000" cy="9144000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing24.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -563,7 +687,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing25.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -593,7 +717,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing26.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -632,7 +756,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="12192000" cy="9144000"/>
+    <ext cx="9915525" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -662,7 +786,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="12192000" cy="9144000"/>
+    <ext cx="10096500" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -692,7 +816,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="12192000" cy="9144000"/>
+    <ext cx="9915525" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -722,7 +846,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="12192000" cy="9144000"/>
+    <ext cx="9915525" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -752,7 +876,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="12192000" cy="9144000"/>
+    <ext cx="9915525" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -782,7 +906,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="12192000" cy="9144000"/>
+    <ext cx="9915525" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -812,7 +936,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="12192000" cy="9144000"/>
+    <ext cx="9915525" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -1122,7 +1246,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1182,22 +1306,22 @@
         <v>49</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>25.15</v>
       </c>
       <c r="D2" t="n">
+        <v>51.38</v>
+      </c>
+      <c r="E2" t="n">
+        <v>32.45918367346939</v>
+      </c>
+      <c r="F2" t="n">
+        <v>32.08</v>
+      </c>
+      <c r="G2" t="n">
         <v>33.2</v>
       </c>
-      <c r="E2" t="n">
-        <v>12.3234693877551</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
       <c r="H2" t="n">
-        <v>15.06547467874539</v>
+        <v>4.087696904908015</v>
       </c>
     </row>
     <row r="3">
@@ -1231,151 +1355,151 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Starting active pores</t>
+          <t>Run read count (millions)</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>49</v>
       </c>
       <c r="C4" t="n">
-        <v>2640</v>
+        <v>1.314</v>
       </c>
       <c r="D4" t="n">
-        <v>8667</v>
+        <v>9.238</v>
       </c>
       <c r="E4" t="n">
-        <v>6871.673469387755</v>
+        <v>3.341285714285714</v>
       </c>
       <c r="F4" t="n">
-        <v>7115</v>
+        <v>3.199</v>
       </c>
       <c r="G4" t="n">
-        <v>7112</v>
+        <v>1.843</v>
       </c>
       <c r="H4" t="n">
-        <v>1248.502976697745</v>
+        <v>1.492264065662196</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Platform QC active pores</t>
+          <t>Starting active pores</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="C5" t="n">
-        <v>5120</v>
+        <v>2640</v>
       </c>
       <c r="D5" t="n">
-        <v>8684</v>
+        <v>8667</v>
       </c>
       <c r="E5" t="n">
-        <v>7167.52</v>
+        <v>6871.673469387755</v>
       </c>
       <c r="F5" t="n">
-        <v>7504</v>
+        <v>7115</v>
       </c>
       <c r="G5" t="n">
-        <v>8684</v>
+        <v>7112</v>
       </c>
       <c r="H5" t="n">
-        <v>968.900068806548</v>
+        <v>1248.502976697745</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Pore difference</t>
+          <t>Platform QC active pores</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>25</v>
       </c>
       <c r="C6" t="n">
-        <v>55</v>
+        <v>5120</v>
       </c>
       <c r="D6" t="n">
-        <v>3751</v>
+        <v>8684</v>
       </c>
       <c r="E6" t="n">
-        <v>731.6799999999999</v>
+        <v>7167.52</v>
       </c>
       <c r="F6" t="n">
-        <v>576</v>
+        <v>7504</v>
       </c>
       <c r="G6" t="n">
-        <v>657</v>
+        <v>8684</v>
       </c>
       <c r="H6" t="n">
-        <v>706.0248295917078</v>
+        <v>968.900068806548</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Flow cells per experiment</t>
+          <t>Pore difference</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>3751</v>
       </c>
       <c r="E7" t="n">
-        <v>1.020833333333333</v>
+        <v>731.6799999999999</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>576</v>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>657</v>
       </c>
       <c r="H7" t="n">
-        <v>0.1443375672974064</v>
+        <v>706.0248295917078</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Flow cell output (Gb)</t>
+          <t>Flow cells per experiment</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" t="n">
-        <v>18.653</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>105.651</v>
+        <v>2</v>
       </c>
       <c r="E8" t="n">
-        <v>60.48742857142857</v>
+        <v>1.020833333333333</v>
       </c>
       <c r="F8" t="n">
-        <v>64.84</v>
+        <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>70.04000000000001</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>23.57373106429414</v>
+        <v>0.1443375672974064</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Total experiment output (Gb)</t>
+          <t>Flow cell output (Gb)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C9" t="n">
         <v>18.653</v>
@@ -1384,75 +1508,103 @@
         <v>105.651</v>
       </c>
       <c r="E9" t="n">
+        <v>60.48742857142857</v>
+      </c>
+      <c r="F9" t="n">
+        <v>64.84</v>
+      </c>
+      <c r="G9" t="n">
+        <v>70.04000000000001</v>
+      </c>
+      <c r="H9" t="n">
+        <v>23.57373106429414</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Total experiment output (Gb)</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>48</v>
+      </c>
+      <c r="C10" t="n">
+        <v>18.653</v>
+      </c>
+      <c r="D10" t="n">
+        <v>105.651</v>
+      </c>
+      <c r="E10" t="n">
         <v>61.74758333333333</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F10" t="n">
         <v>65.8455</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G10" t="n">
         <v>51.4</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H10" t="n">
         <v>23.22835168480337</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
         <is>
           <t>Flow Cells</t>
         </is>
       </c>
-      <c r="B11" s="1" t="inlineStr">
+      <c r="B12" s="1" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>1</v>
-      </c>
-      <c r="B12" t="n">
-        <v>47</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
         <v>2</v>
       </c>
-      <c r="B13" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
         <is>
           <t>MinKNOW Version</t>
         </is>
       </c>
-      <c r="B15" s="1" t="inlineStr">
+      <c r="B16" s="1" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>22.10.7</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>29</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>22.10.7</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
           <t>23.11.7</t>
         </is>
       </c>
-      <c r="B17" t="n">
+      <c r="B18" t="n">
         <v>20</v>
       </c>
     </row>
@@ -2518,6 +2670,82 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
Updated example tutorial files to reflect newest parser and dashboard thus far
</commit_message>
<xml_diff>
--- a/example_summary_spreadsheet.xlsx
+++ b/example_summary_spreadsheet.xlsx
@@ -1246,7 +1246,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1312,7 +1312,7 @@
         <v>51.38</v>
       </c>
       <c r="E2" t="n">
-        <v>32.45918367346939</v>
+        <v>32.459</v>
       </c>
       <c r="F2" t="n">
         <v>32.08</v>
@@ -1321,7 +1321,7 @@
         <v>33.2</v>
       </c>
       <c r="H2" t="n">
-        <v>4.087696904908015</v>
+        <v>4.046</v>
       </c>
     </row>
     <row r="3">
@@ -1340,7 +1340,7 @@
         <v>105.651</v>
       </c>
       <c r="E3" t="n">
-        <v>60.48742857142857</v>
+        <v>60.487</v>
       </c>
       <c r="F3" t="n">
         <v>64.84</v>
@@ -1349,7 +1349,7 @@
         <v>99.94799999999999</v>
       </c>
       <c r="H3" t="n">
-        <v>23.57373106429414</v>
+        <v>23.332</v>
       </c>
     </row>
     <row r="4">
@@ -1368,7 +1368,7 @@
         <v>9.238</v>
       </c>
       <c r="E4" t="n">
-        <v>3.341285714285714</v>
+        <v>3.341</v>
       </c>
       <c r="F4" t="n">
         <v>3.199</v>
@@ -1377,7 +1377,7 @@
         <v>1.843</v>
       </c>
       <c r="H4" t="n">
-        <v>1.492264065662196</v>
+        <v>1.477</v>
       </c>
     </row>
     <row r="5">
@@ -1396,7 +1396,7 @@
         <v>8667</v>
       </c>
       <c r="E5" t="n">
-        <v>6871.673469387755</v>
+        <v>6871.673</v>
       </c>
       <c r="F5" t="n">
         <v>7115</v>
@@ -1405,129 +1405,129 @@
         <v>7112</v>
       </c>
       <c r="H5" t="n">
-        <v>1248.502976697745</v>
+        <v>1235.697</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Platform QC active pores</t>
+          <t>Average active pores</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="C6" t="n">
-        <v>5120</v>
+        <v>830.457</v>
       </c>
       <c r="D6" t="n">
-        <v>8684</v>
+        <v>3862.375</v>
       </c>
       <c r="E6" t="n">
-        <v>7167.52</v>
+        <v>2296.343</v>
       </c>
       <c r="F6" t="n">
-        <v>7504</v>
+        <v>2342.022</v>
       </c>
       <c r="G6" t="n">
-        <v>8684</v>
+        <v>3113.067</v>
       </c>
       <c r="H6" t="n">
-        <v>968.900068806548</v>
+        <v>718.3680000000001</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Pore difference</t>
+          <t>Platform QC active pores</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>25</v>
       </c>
       <c r="C7" t="n">
-        <v>55</v>
+        <v>5120</v>
       </c>
       <c r="D7" t="n">
-        <v>3751</v>
+        <v>8684</v>
       </c>
       <c r="E7" t="n">
-        <v>731.6799999999999</v>
+        <v>7167.52</v>
       </c>
       <c r="F7" t="n">
-        <v>576</v>
+        <v>7504</v>
       </c>
       <c r="G7" t="n">
-        <v>657</v>
+        <v>8684</v>
       </c>
       <c r="H7" t="n">
-        <v>706.0248295917078</v>
+        <v>949.324</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Flow cells per experiment</t>
+          <t>Pore difference</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>3751</v>
       </c>
       <c r="E8" t="n">
-        <v>1.020833333333333</v>
+        <v>731.6799999999999</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>576</v>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>657</v>
       </c>
       <c r="H8" t="n">
-        <v>0.1443375672974064</v>
+        <v>691.76</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Flow cell output (Gb)</t>
+          <t>Flow cells per experiment</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" t="n">
-        <v>18.653</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>105.651</v>
+        <v>2</v>
       </c>
       <c r="E9" t="n">
-        <v>60.48742857142857</v>
+        <v>1.021</v>
       </c>
       <c r="F9" t="n">
-        <v>64.84</v>
+        <v>1</v>
       </c>
       <c r="G9" t="n">
-        <v>70.04000000000001</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>23.57373106429414</v>
+        <v>0.143</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Total experiment output (Gb)</t>
+          <t>Flow cell output (Gb)</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C10" t="n">
         <v>18.653</v>
@@ -1536,75 +1536,359 @@
         <v>105.651</v>
       </c>
       <c r="E10" t="n">
-        <v>61.74758333333333</v>
+        <v>60.487</v>
       </c>
       <c r="F10" t="n">
-        <v>65.8455</v>
+        <v>64.84</v>
       </c>
       <c r="G10" t="n">
+        <v>70.04000000000001</v>
+      </c>
+      <c r="H10" t="n">
+        <v>23.332</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Total experiment output (Gb)</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>48</v>
+      </c>
+      <c r="C11" t="n">
+        <v>18.653</v>
+      </c>
+      <c r="D11" t="n">
+        <v>105.651</v>
+      </c>
+      <c r="E11" t="n">
+        <v>61.748</v>
+      </c>
+      <c r="F11" t="n">
+        <v>65.846</v>
+      </c>
+      <c r="G11" t="n">
         <v>51.4</v>
       </c>
-      <c r="H10" t="n">
-        <v>23.22835168480337</v>
+      <c r="H11" t="n">
+        <v>22.985</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Flow Cells</t>
-        </is>
-      </c>
-      <c r="B12" s="1" t="inlineStr">
-        <is>
-          <t>Frequency</t>
-        </is>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Active pore AUC</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>49</v>
+      </c>
+      <c r="C12" t="n">
+        <v>33470</v>
+      </c>
+      <c r="D12" t="n">
+        <v>165620</v>
+      </c>
+      <c r="E12" t="n">
+        <v>96840.49000000001</v>
+      </c>
+      <c r="F12" t="n">
+        <v>99200</v>
+      </c>
+      <c r="G12" t="n">
+        <v>140088</v>
+      </c>
+      <c r="H12" t="n">
+        <v>35501.966</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>1</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Starting pore occupancy</t>
+        </is>
       </c>
       <c r="B13" t="n">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="C13" t="n">
+        <v>77.384</v>
+      </c>
+      <c r="D13" t="n">
+        <v>98.373</v>
+      </c>
+      <c r="E13" t="n">
+        <v>91.792</v>
+      </c>
+      <c r="F13" t="n">
+        <v>93.358</v>
+      </c>
+      <c r="G13" t="n">
+        <v>95.548</v>
+      </c>
+      <c r="H13" t="n">
+        <v>4.999</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>2</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Average pore occupancy</t>
+        </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>49</v>
+      </c>
+      <c r="C14" t="n">
+        <v>73.00700000000001</v>
+      </c>
+      <c r="D14" t="n">
+        <v>96.39100000000001</v>
+      </c>
+      <c r="E14" t="n">
+        <v>90.52200000000001</v>
+      </c>
+      <c r="F14" t="n">
+        <v>91.485</v>
+      </c>
+      <c r="G14" t="n">
+        <v>96.39100000000001</v>
+      </c>
+      <c r="H14" t="n">
+        <v>5.14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Passed modal Q score</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>MinKNOW Version</t>
-        </is>
-      </c>
-      <c r="B16" s="1" t="inlineStr">
-        <is>
-          <t>Frequency</t>
-        </is>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Failed modal Q score</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>22.10.7</t>
+          <t>Starting translocation speed</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>Average translocation speed</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Starting median Q score</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Average median Q score</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Passed bases (Gb)</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>29</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Failed bases (Gb)</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>29</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Percentage passed bases</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>29</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>Flow Cells</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>Frequency</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>1</v>
+      </c>
+      <c r="B26" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>MinKNOW Version</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>Frequency</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>22.10.7</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
           <t>23.11.7</t>
         </is>
       </c>
-      <c r="B18" t="n">
+      <c r="B31" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>Sample Rate (Hz)</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>Frequency</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>4000</v>
+      </c>
+      <c r="B34" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B35" t="n">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new 1D violin/swarmplots showing distributions of additional metrics
</commit_message>
<xml_diff>
--- a/example_summary_spreadsheet.xlsx
+++ b/example_summary_spreadsheet.xlsx
@@ -13,28 +13,35 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Run data output plot" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Run read count plot" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Starting active pores plot" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Flow cells per experiment plot" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Output per experiment plot" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Output per flow cell plot" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform QC active pores plot" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform-seq pore diff plot" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform-seq time diff plot" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pores vs. data output" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pores vs. read count" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pores vs. read N50" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 vs. data output" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 vs. data no line" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 vs. read count" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 vs. count no line" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. starting active pores" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. pore difference" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore vs. time difference" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference vs. run output" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output pore diff" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output starting pores" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform QC pores over time" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference over time" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Run output over time" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Average active pores plot" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pore AUC plot" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Starting pore occupancy plot" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Average pore occupancy plot" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Passed bases plot" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Failed bases plot" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Percentage passed bases plot" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Flow cells per experiment plot" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Output per experiment plot" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Output per flow cell plot" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform QC active pores plot" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform-seq pore diff plot" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform-seq time diff plot" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pores vs. data output" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pores vs. read count" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pores vs. read N50" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 vs. data output" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 vs. data no line" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 vs. read count" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 vs. count no line" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. starting active pores" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. pore difference" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore vs. time difference" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference vs. run output" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output pore diff" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output starting pores" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform QC pores over time" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference over time" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Run output over time" sheetId="36" state="visible" r:id="rId36"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -246,7 +253,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8153400" cy="6457950"/>
+    <ext cx="9915525" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -276,7 +283,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="7905750" cy="6457950"/>
+    <ext cx="9915525" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -306,7 +313,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8029575" cy="6457950"/>
+    <ext cx="9915525" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -328,6 +335,126 @@
 </file>
 
 <file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="9915525" cy="8648700"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="9915525" cy="8648700"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="9915525" cy="8648700"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="9915525" cy="8648700"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -357,37 +484,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="8153400" cy="6457950"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -397,96 +494,6 @@
       <rowOff>0</rowOff>
     </from>
     <ext cx="7905750" cy="6457950"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="7905750" cy="6457950"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="8277225" cy="6457950"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="8277225" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -546,7 +553,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8277225" cy="6457950"/>
+    <ext cx="8029575" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -606,7 +613,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8191500" cy="6457950"/>
+    <ext cx="8153400" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -636,7 +643,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8191500" cy="6457950"/>
+    <ext cx="7905750" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -666,7 +673,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8467725" cy="6991350"/>
+    <ext cx="7905750" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -696,7 +703,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8467725" cy="6991350"/>
+    <ext cx="8277225" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -726,7 +733,97 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8153400" cy="6991350"/>
+    <ext cx="8277225" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing27.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8277225" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing28.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8153400" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing29.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8191500" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -777,6 +874,126 @@
 </wsDr>
 </file>
 
+<file path=xl/drawings/drawing30.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8191500" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing31.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8467725" cy="6991350"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing32.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8467725" cy="6991350"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing33.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8153400" cy="6991350"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
@@ -846,7 +1063,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9915525" cy="8648700"/>
+    <ext cx="10058400" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -3708,6 +3925,139 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Updated tutorial sample outputs and further debugging of dashboard generator
</commit_message>
<xml_diff>
--- a/example_summary_spreadsheet.xlsx
+++ b/example_summary_spreadsheet.xlsx
@@ -33,15 +33,22 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 vs. data no line" sheetId="25" state="visible" r:id="rId25"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 vs. read count" sheetId="26" state="visible" r:id="rId26"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read N50 vs. count no line" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. starting active pores" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. pore difference" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore vs. time difference" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference vs. run output" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output pore diff" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output starting pores" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform QC pores over time" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference over time" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Run output over time" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Start vs. avg active pores" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Start active pores vs. AUC" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Avg active pores vs. data" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pore AUC vs. data" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Avg pore occup. vs. data" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. starting active pores" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. pore difference" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore vs. time difference" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference vs. run output" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore diff. vs. active pore AUC" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore occup. vs. pore diff." sheetId="38" state="visible" r:id="rId38"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output pore diff" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output starting pores" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform QC pores over time" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference over time" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Run output over time" sheetId="43" state="visible" r:id="rId43"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -733,7 +740,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8277225" cy="6457950"/>
+    <ext cx="8534400" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -763,7 +770,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8277225" cy="6457950"/>
+    <ext cx="8382000" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -823,7 +830,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8191500" cy="6457950"/>
+    <ext cx="8153400" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -883,6 +890,186 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
+    <ext cx="8277225" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing31.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8277225" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing32.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8277225" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing33.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8153400" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing34.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8534400" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing35.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8277225" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing36.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
     <ext cx="8191500" cy="6457950"/>
     <pic>
       <nvPicPr>
@@ -904,7 +1091,37 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing37.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8191500" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing38.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -934,7 +1151,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing39.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -964,7 +1181,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -973,7 +1190,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8153400" cy="6991350"/>
+    <ext cx="10096500" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -994,7 +1211,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing40.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -1003,7 +1220,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="10096500" cy="8648700"/>
+    <ext cx="8153400" cy="6991350"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -4058,7 +4275,140 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
Newest version of dashboard generator with updated run type designation and options to print summary table with platform qc and/or run type info
</commit_message>
<xml_diff>
--- a/example_summary_spreadsheet.xlsx
+++ b/example_summary_spreadsheet.xlsx
@@ -37,18 +37,19 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Start active pores vs. AUC" sheetId="29" state="visible" r:id="rId29"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Avg active pores vs. data" sheetId="30" state="visible" r:id="rId30"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pore AUC vs. data" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Avg pore occup. vs. data" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. starting active pores" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. pore difference" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore vs. time difference" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference vs. run output" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore diff. vs. active pore AUC" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore occup. vs. pore diff." sheetId="38" state="visible" r:id="rId38"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output pore diff" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output starting pores" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform QC pores over time" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference over time" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Run output over time" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore AUC vs. read count" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Avg pore occup. vs. data" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. starting active pores" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. pore difference" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore vs. time difference" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference vs. run output" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore diff. vs. active pore AUC" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore occup. vs. pore diff." sheetId="39" state="visible" r:id="rId39"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output pore diff" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output starting pores" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform QC pores over time" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference over time" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Run output over time" sheetId="44" state="visible" r:id="rId44"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -830,7 +831,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8153400" cy="6457950"/>
+    <ext cx="7905750" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -890,7 +891,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8277225" cy="6457950"/>
+    <ext cx="8153400" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -980,6 +981,36 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
+    <ext cx="8277225" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing34.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
     <ext cx="8153400" cy="6457950"/>
     <pic>
       <nvPicPr>
@@ -1001,7 +1032,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing35.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -1031,7 +1062,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing36.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -1041,36 +1072,6 @@
       <rowOff>0</rowOff>
     </from>
     <ext cx="8277225" cy="6457950"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing36.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="8191500" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -1130,7 +1131,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8467725" cy="6991350"/>
+    <ext cx="8191500" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -1212,6 +1213,36 @@
 </file>
 
 <file path=xl/drawings/drawing40.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8467725" cy="6991350"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing41.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -1752,7 +1783,7 @@
         <v>32.08</v>
       </c>
       <c r="G2" t="n">
-        <v>33.2</v>
+        <v>33.13</v>
       </c>
       <c r="H2" t="n">
         <v>4.046</v>
@@ -1780,7 +1811,7 @@
         <v>64.84</v>
       </c>
       <c r="G3" t="n">
-        <v>99.94799999999999</v>
+        <v>44.76</v>
       </c>
       <c r="H3" t="n">
         <v>23.332</v>
@@ -1836,7 +1867,7 @@
         <v>7115</v>
       </c>
       <c r="G5" t="n">
-        <v>7112</v>
+        <v>7804</v>
       </c>
       <c r="H5" t="n">
         <v>1235.697</v>
@@ -1864,7 +1895,7 @@
         <v>2342.022</v>
       </c>
       <c r="G6" t="n">
-        <v>3113.067</v>
+        <v>1606.787</v>
       </c>
       <c r="H6" t="n">
         <v>718.3680000000001</v>
@@ -2032,7 +2063,7 @@
         <v>99200</v>
       </c>
       <c r="G12" t="n">
-        <v>140088</v>
+        <v>75519</v>
       </c>
       <c r="H12" t="n">
         <v>35501.966</v>
@@ -2060,7 +2091,7 @@
         <v>93.358</v>
       </c>
       <c r="G13" t="n">
-        <v>95.548</v>
+        <v>86.22799999999999</v>
       </c>
       <c r="H13" t="n">
         <v>4.999</v>
@@ -2088,7 +2119,7 @@
         <v>91.485</v>
       </c>
       <c r="G14" t="n">
-        <v>96.39100000000001</v>
+        <v>88.922</v>
       </c>
       <c r="H14" t="n">
         <v>5.14</v>
@@ -2548,7 +2579,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Top up</t>
+          <t>Run type</t>
         </is>
       </c>
     </row>
@@ -2563,7 +2594,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2578,7 +2609,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2593,7 +2624,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2608,7 +2639,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2623,7 +2654,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2638,7 +2669,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2653,7 +2684,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2668,7 +2699,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2683,7 +2714,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2698,7 +2729,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2713,7 +2744,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2728,7 +2759,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2743,7 +2774,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2758,7 +2789,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2773,7 +2804,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2788,7 +2819,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2803,7 +2834,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2818,7 +2849,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2833,7 +2864,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2848,7 +2879,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2863,7 +2894,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2878,7 +2909,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2893,7 +2924,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2908,7 +2939,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2938,7 +2969,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2953,7 +2984,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2968,7 +2999,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2983,7 +3014,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -2998,7 +3029,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -3118,7 +3149,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -3133,7 +3164,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -3148,7 +3179,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -3163,7 +3194,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -3178,7 +3209,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -3193,7 +3224,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -3223,7 +3254,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -3238,7 +3269,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -3253,7 +3284,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -3268,7 +3299,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -3283,7 +3314,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
     </row>
@@ -4409,6 +4440,25 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>